<commit_message>
added support for keywords
</commit_message>
<xml_diff>
--- a/TestCaseImporter/testcases.xlsx
+++ b/TestCaseImporter/testcases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aderthad\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aderthad\Bitnami\apps\testlink\htdocs\plugins\TestCaseImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
@@ -23,6 +23,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author/>
+    <author>Aderthad</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0">
@@ -50,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,6 +98,30 @@
             <charset val="238"/>
           </rPr>
           <t>1 (Low), 2 (Medium), 3 (High)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aderthad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Multiple keywords can be separeted by a comma (,)</t>
         </r>
       </text>
     </comment>
@@ -155,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="99">
   <si>
     <t>Test suite name</t>
   </si>
@@ -163,9 +188,6 @@
     <t>Test suite details</t>
   </si>
   <si>
-    <t>TC number</t>
-  </si>
-  <si>
     <t>TC Name</t>
   </si>
   <si>
@@ -443,13 +465,25 @@
   </si>
   <si>
     <t>ReqDoc2</t>
+  </si>
+  <si>
+    <t>Keywords</t>
+  </si>
+  <si>
+    <t>keyword</t>
+  </si>
+  <si>
+    <t>keywords</t>
+  </si>
+  <si>
+    <t>keyword2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -464,13 +498,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b/>
@@ -494,6 +521,19 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -540,15 +580,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -557,7 +594,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -661,7 +698,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -710,7 +747,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -759,7 +796,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -808,7 +845,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -857,7 +894,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1202,19 +1239,18 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625"/>
-    <col min="2" max="2" width="24.140625"/>
-    <col min="3" max="3" width="9.7109375"/>
-    <col min="4" max="4" width="17.85546875"/>
-    <col min="5" max="5" width="19.140625"/>
-    <col min="6" max="6" width="26.85546875"/>
-    <col min="7" max="7" width="13.5703125"/>
-    <col min="8" max="8" width="10.42578125"/>
+    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875"/>
+    <col min="6" max="6" width="13.5703125"/>
+    <col min="7" max="8" width="11.5703125" customWidth="1"/>
     <col min="9" max="9" width="32.7109375"/>
     <col min="10" max="10" width="23.85546875"/>
     <col min="11" max="12" width="13.140625"/>
@@ -1235,510 +1271,525 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
+      <c r="H2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>18</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4" t="s">
         <v>20</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
       <c r="L4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="J5" t="s">
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6" t="s">
         <v>26</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" t="s">
-        <v>28</v>
-      </c>
       <c r="L6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="O6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" t="s">
         <v>31</v>
-      </c>
-      <c r="J8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
         <v>33</v>
-      </c>
-      <c r="J9" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="I12" t="s">
         <v>38</v>
       </c>
-      <c r="G12">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>3</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>39</v>
-      </c>
-      <c r="J12" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
         <v>41</v>
-      </c>
-      <c r="J13" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I14" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" t="s">
         <v>43</v>
       </c>
-      <c r="J14" t="s">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
         <v>38</v>
       </c>
-      <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>39</v>
-      </c>
-      <c r="J15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I16" t="s">
+        <v>45</v>
+      </c>
+      <c r="J16" t="s">
         <v>46</v>
-      </c>
-      <c r="J16" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
-        <v>52</v>
+      <c r="H19" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="B20" t="s">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
         <v>55</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
         <v>56</v>
       </c>
-      <c r="G21">
-        <v>1</v>
-      </c>
-      <c r="H21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>57</v>
-      </c>
-      <c r="J21" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>61</v>
       </c>
-      <c r="E24" t="s">
-        <v>62</v>
+      <c r="F24">
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1</v>
-      </c>
-      <c r="H24">
         <v>2</v>
       </c>
+      <c r="H24" t="s">
+        <v>98</v>
+      </c>
       <c r="I24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J24" t="s">
         <v>57</v>
-      </c>
-      <c r="J24" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J27" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
         <v>64</v>
       </c>
-      <c r="B30" t="s">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>66</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="I31" t="s">
         <v>67</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>2</v>
-      </c>
-      <c r="I31" t="s">
-        <v>68</v>
-      </c>
       <c r="J31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I32" t="s">
+        <v>68</v>
+      </c>
+      <c r="J32" t="s">
         <v>69</v>
-      </c>
-      <c r="J32" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>70</v>
+      </c>
+      <c r="B33" t="s">
         <v>71</v>
       </c>
-      <c r="B33" t="s">
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>73</v>
       </c>
-      <c r="E34" t="s">
-        <v>74</v>
+      <c r="F34">
+        <v>1</v>
       </c>
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
       <c r="I34" t="s">
+        <v>73</v>
+      </c>
+      <c r="J34" t="s">
         <v>74</v>
       </c>
-      <c r="J34" t="s">
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>76</v>
       </c>
-      <c r="E35" t="s">
-        <v>77</v>
+      <c r="F35">
+        <v>1</v>
       </c>
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
       <c r="I35" t="s">
+        <v>76</v>
+      </c>
+      <c r="J35" t="s">
         <v>77</v>
       </c>
-      <c r="J35" t="s">
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>79</v>
       </c>
-      <c r="E36" t="s">
-        <v>80</v>
+      <c r="F36">
+        <v>1</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
       <c r="I36" t="s">
+        <v>79</v>
+      </c>
+      <c r="J36" t="s">
         <v>80</v>
       </c>
-      <c r="J36" t="s">
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>82</v>
       </c>
-      <c r="E37" t="s">
-        <v>83</v>
+      <c r="F37">
+        <v>1</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
       <c r="I37" t="s">
+        <v>82</v>
+      </c>
+      <c r="J37" t="s">
         <v>83</v>
       </c>
-      <c r="J37" t="s">
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>85</v>
       </c>
-      <c r="E38" t="s">
-        <v>86</v>
+      <c r="F38">
+        <v>1</v>
       </c>
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="H38">
-        <v>1</v>
-      </c>
       <c r="I38" t="s">
+        <v>85</v>
+      </c>
+      <c r="J38" t="s">
         <v>86</v>
       </c>
-      <c r="J38" t="s">
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>88</v>
       </c>
-      <c r="E39" t="s">
-        <v>89</v>
+      <c r="F39">
+        <v>1</v>
       </c>
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
       <c r="I39" t="s">
+        <v>88</v>
+      </c>
+      <c r="J39" t="s">
         <v>89</v>
-      </c>
-      <c r="J39" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added TC status and exp exec time columns to the templates.
</commit_message>
<xml_diff>
--- a/TestCaseImporter/testcases.xlsx
+++ b/TestCaseImporter/testcases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -51,7 +51,37 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aderthad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1 - Draft (default)
+2 - Ready for review
+3 - Review in progress
+4 - Rework
+5 - Obsolete
+6 - Future
+7 - Final</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -76,7 +106,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="H1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +131,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="1" shapeId="0">
+    <comment ref="I1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Aderthad:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Estimated exec. duration (min)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,37 +204,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>marcu_000:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="238"/>
-          </rPr>
-          <t>Document IDs covered by this test case. Multiple document IDs can be separated by semi-comma (;)</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
   <si>
     <t>Test suite name</t>
   </si>
@@ -474,6 +503,12 @@
   </si>
   <si>
     <t>keyword, keyword2</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Duration</t>
   </si>
 </sst>
 </file>
@@ -695,7 +730,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -744,7 +779,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -793,7 +828,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -842,7 +877,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -891,7 +926,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1232,11 +1267,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,16 +1281,18 @@
     <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
     <col min="5" max="5" width="26.85546875"/>
-    <col min="6" max="6" width="13.5703125"/>
-    <col min="7" max="8" width="11.5703125" customWidth="1"/>
-    <col min="9" max="9" width="32.7109375"/>
-    <col min="10" max="10" width="23.85546875"/>
-    <col min="11" max="12" width="13.140625"/>
-    <col min="13" max="13" width="9.7109375"/>
-    <col min="16" max="1023" width="8.5703125"/>
+    <col min="7" max="7" width="13.5703125"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="32.7109375"/>
+    <col min="12" max="12" width="23.85546875"/>
+    <col min="13" max="14" width="13.140625"/>
+    <col min="15" max="15" width="9.7109375"/>
+    <col min="18" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,48 +1309,54 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1321,7 +1364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>17</v>
       </c>
@@ -1331,95 +1374,95 @@
       <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>1</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>21</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>91</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>93</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I5" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
         <v>22</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>24</v>
       </c>
       <c r="D6" t="s">
         <v>25</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>26</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>27</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>92</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>94</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I7" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
         <v>28</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I8" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
         <v>30</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I9" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
         <v>32</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1427,79 +1470,79 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>36</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>3</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>38</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
         <v>40</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
         <v>42</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>44</v>
       </c>
       <c r="D15" t="s">
         <v>37</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>2</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>3</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>38</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I16" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
         <v>45</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I17" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
         <v>42</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -1507,7 +1550,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -1515,108 +1558,108 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>52</v>
       </c>
       <c r="B20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>55</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>1</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>2</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>56</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I22" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
         <v>58</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I23" t="s">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
         <v>22</v>
       </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>60</v>
       </c>
       <c r="D24" t="s">
         <v>61</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>1</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>2</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>56</v>
       </c>
-      <c r="J24" t="s">
+      <c r="L24" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I25" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
         <v>58</v>
       </c>
-      <c r="J25" t="s">
+      <c r="L25" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I26" t="s">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
         <v>62</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I27" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
         <v>22</v>
       </c>
-      <c r="J27" t="s">
+      <c r="L27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1624,35 +1667,35 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>65</v>
       </c>
       <c r="D31" t="s">
         <v>66</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>1</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>2</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>67</v>
       </c>
-      <c r="J31" t="s">
+      <c r="L31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I32" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
         <v>68</v>
       </c>
-      <c r="J32" t="s">
+      <c r="L32" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>70</v>
       </c>
@@ -1660,129 +1703,129 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>72</v>
       </c>
       <c r="D34" t="s">
         <v>73</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
       <c r="G34">
         <v>1</v>
       </c>
-      <c r="I34" t="s">
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
         <v>73</v>
       </c>
-      <c r="J34" t="s">
+      <c r="L34" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>75</v>
       </c>
       <c r="D35" t="s">
         <v>76</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
       <c r="G35">
         <v>1</v>
       </c>
-      <c r="I35" t="s">
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
         <v>76</v>
       </c>
-      <c r="J35" t="s">
+      <c r="L35" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>78</v>
       </c>
       <c r="D36" t="s">
         <v>79</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
       <c r="G36">
         <v>1</v>
       </c>
-      <c r="I36" t="s">
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
         <v>79</v>
       </c>
-      <c r="J36" t="s">
+      <c r="L36" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>81</v>
       </c>
       <c r="D37" t="s">
         <v>82</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
       <c r="G37">
         <v>1</v>
       </c>
-      <c r="I37" t="s">
+      <c r="H37">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
         <v>82</v>
       </c>
-      <c r="J37" t="s">
+      <c r="L37" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>84</v>
       </c>
       <c r="D38" t="s">
         <v>85</v>
       </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
       <c r="G38">
         <v>1</v>
       </c>
-      <c r="I38" t="s">
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="K38" t="s">
         <v>85</v>
       </c>
-      <c r="J38" t="s">
+      <c r="L38" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>87</v>
       </c>
       <c r="D39" t="s">
         <v>88</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
       <c r="G39">
         <v>1</v>
       </c>
-      <c r="I39" t="s">
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="K39" t="s">
         <v>88</v>
       </c>
-      <c r="J39" t="s">
+      <c r="L39" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N39 M1 J2:J32 M24:M39">
+    <dataValidation operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P1:P39 O1 L2:L32 O24:O39">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Changed TC Name column name to Test case name.
</commit_message>
<xml_diff>
--- a/TestCaseImporter/testcases.xlsx
+++ b/TestCaseImporter/testcases.xlsx
@@ -217,9 +217,6 @@
     <t>Test suite details</t>
   </si>
   <si>
-    <t>TC Name</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>Duration</t>
+  </si>
+  <si>
+    <t>Test case name</t>
   </si>
 </sst>
 </file>
@@ -1271,7 +1271,7 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,79 +1300,79 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>7</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
       <c r="J2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -1381,35 +1381,35 @@
         <v>2</v>
       </c>
       <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
         <v>20</v>
       </c>
-      <c r="L4" t="s">
-        <v>21</v>
-      </c>
       <c r="N4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" t="s">
         <v>22</v>
-      </c>
-      <c r="L5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -1418,64 +1418,64 @@
         <v>2</v>
       </c>
       <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="L6" t="s">
-        <v>27</v>
-      </c>
       <c r="N6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="O6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="Q6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
         <v>28</v>
-      </c>
-      <c r="L7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" t="s">
         <v>30</v>
-      </c>
-      <c r="L8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K9" t="s">
+        <v>31</v>
+      </c>
+      <c r="L9" t="s">
         <v>32</v>
-      </c>
-      <c r="L9" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
         <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
       </c>
       <c r="G12">
         <v>2</v>
@@ -1484,34 +1484,34 @@
         <v>3</v>
       </c>
       <c r="K12" t="s">
+        <v>37</v>
+      </c>
+      <c r="L12" t="s">
         <v>38</v>
-      </c>
-      <c r="L12" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K13" t="s">
+        <v>39</v>
+      </c>
+      <c r="L13" t="s">
         <v>40</v>
-      </c>
-      <c r="L13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K14" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" t="s">
         <v>42</v>
-      </c>
-      <c r="L14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G15">
         <v>2</v>
@@ -1520,61 +1520,61 @@
         <v>3</v>
       </c>
       <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" t="s">
         <v>38</v>
-      </c>
-      <c r="L15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="K16" t="s">
+        <v>44</v>
+      </c>
+      <c r="L16" t="s">
         <v>45</v>
-      </c>
-      <c r="L16" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
         <v>48</v>
-      </c>
-      <c r="B18" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
         <v>50</v>
-      </c>
-      <c r="B19" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
       <c r="J20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
         <v>54</v>
-      </c>
-      <c r="D21" t="s">
-        <v>55</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1583,34 +1583,34 @@
         <v>2</v>
       </c>
       <c r="K21" t="s">
+        <v>55</v>
+      </c>
+      <c r="L21" t="s">
         <v>56</v>
-      </c>
-      <c r="L21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
         <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>61</v>
       </c>
       <c r="G24">
         <v>1</v>
@@ -1619,60 +1619,60 @@
         <v>2</v>
       </c>
       <c r="K24" t="s">
+        <v>55</v>
+      </c>
+      <c r="L24" t="s">
         <v>56</v>
-      </c>
-      <c r="L24" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" t="s">
         <v>63</v>
-      </c>
-      <c r="B30" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" t="s">
         <v>65</v>
-      </c>
-      <c r="D31" t="s">
-        <v>66</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -1681,34 +1681,34 @@
         <v>2</v>
       </c>
       <c r="K31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K32" t="s">
+        <v>67</v>
+      </c>
+      <c r="L32" t="s">
         <v>68</v>
-      </c>
-      <c r="L32" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
         <v>70</v>
-      </c>
-      <c r="B33" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>71</v>
+      </c>
+      <c r="D34" t="s">
         <v>72</v>
-      </c>
-      <c r="D34" t="s">
-        <v>73</v>
       </c>
       <c r="G34">
         <v>1</v>
@@ -1717,18 +1717,18 @@
         <v>1</v>
       </c>
       <c r="K34" t="s">
+        <v>72</v>
+      </c>
+      <c r="L34" t="s">
         <v>73</v>
-      </c>
-      <c r="L34" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" t="s">
         <v>75</v>
-      </c>
-      <c r="D35" t="s">
-        <v>76</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -1737,18 +1737,18 @@
         <v>1</v>
       </c>
       <c r="K35" t="s">
+        <v>75</v>
+      </c>
+      <c r="L35" t="s">
         <v>76</v>
-      </c>
-      <c r="L35" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
         <v>78</v>
-      </c>
-      <c r="D36" t="s">
-        <v>79</v>
       </c>
       <c r="G36">
         <v>1</v>
@@ -1757,18 +1757,18 @@
         <v>1</v>
       </c>
       <c r="K36" t="s">
+        <v>78</v>
+      </c>
+      <c r="L36" t="s">
         <v>79</v>
-      </c>
-      <c r="L36" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" t="s">
         <v>81</v>
-      </c>
-      <c r="D37" t="s">
-        <v>82</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -1777,18 +1777,18 @@
         <v>1</v>
       </c>
       <c r="K37" t="s">
+        <v>81</v>
+      </c>
+      <c r="L37" t="s">
         <v>82</v>
-      </c>
-      <c r="L37" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
+        <v>83</v>
+      </c>
+      <c r="D38" t="s">
         <v>84</v>
-      </c>
-      <c r="D38" t="s">
-        <v>85</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1797,18 +1797,18 @@
         <v>1</v>
       </c>
       <c r="K38" t="s">
+        <v>84</v>
+      </c>
+      <c r="L38" t="s">
         <v>85</v>
-      </c>
-      <c r="L38" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
+        <v>86</v>
+      </c>
+      <c r="D39" t="s">
         <v>87</v>
-      </c>
-      <c r="D39" t="s">
-        <v>88</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -1817,10 +1817,10 @@
         <v>1</v>
       </c>
       <c r="K39" t="s">
+        <v>87</v>
+      </c>
+      <c r="L39" t="s">
         <v>88</v>
-      </c>
-      <c r="L39" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>